<commit_message>
added universe and type_allowed
</commit_message>
<xml_diff>
--- a/DerivativeArbitrage/Runtime/configs/static_params.xlsx
+++ b/DerivativeArbitrage/Runtime/configs/static_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\puffin\DerivativeArbitrage\Runtime\Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8255628-57DD-446D-A903-A02C261107EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C36513-7840-44B4-88DF-C9D3362003E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14145" yWindow="1545" windowWidth="27615" windowHeight="17850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19755" yWindow="585" windowWidth="27615" windowHeight="17850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>value</t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>12h</t>
+  </si>
+  <si>
+    <t>UNIVERSE</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>TYPE_ALLOWED</t>
+  </si>
+  <si>
+    <t>perpetual</t>
+  </si>
+  <si>
+    <t>SystematicPerp</t>
+  </si>
+  <si>
+    <t>suybbaccount, filename or number</t>
   </si>
 </sst>
 </file>
@@ -411,17 +429,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,8 +481,11 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1">
-        <v>100000</v>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -524,6 +545,25 @@
       </c>
       <c r="B12">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extend to max universe
</commit_message>
<xml_diff>
--- a/DerivativeArbitrage/Runtime/configs/static_params.xlsx
+++ b/DerivativeArbitrage/Runtime/configs/static_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\puffin\DerivativeArbitrage\Runtime\Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C36513-7840-44B4-88DF-C9D3362003E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CB5159-0453-45B2-B177-E04B7CC72A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19755" yWindow="585" windowWidth="27615" windowHeight="17850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="1980" windowWidth="27615" windowHeight="17850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
minor fixes and features
</commit_message>
<xml_diff>
--- a/DerivativeArbitrage/Runtime/configs/static_params.xlsx
+++ b/DerivativeArbitrage/Runtime/configs/static_params.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\pyCharmProjects\SystematicCeFi\DerivativeArbitrage\Runtime\Configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\pyCharmProjects\SystematicCeFi\DerivativeArbitrage\Runtime\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4C49D6-EF5D-4383-8DAC-4C69160FE1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1803FCCB-9540-4FB7-99CD-02FB98C3436B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>value</t>
   </si>
@@ -96,19 +96,22 @@
     <t>2d</t>
   </si>
   <si>
-    <t>SysPerp</t>
-  </si>
-  <si>
     <t>subaccount, filename or number</t>
   </si>
   <si>
     <t>related to nb underlying * slice size</t>
   </si>
   <si>
+    <t>$BASED+3DOG+AMPL+AUSCM+BASE+BTRFLY+CHEEZ+CLAM+COIL+CROWN+DEBASE+DIGG+DIOS+DITTO+EIGHT+EXOD+FHM+FLOKIN+FOREVERPUMP+FORT+GRM+GRPL+GRV+GRX+GURU+GYRO+HEC+IN+IUP+JADE+KLIMA+LOVE+MARK+META+NMS+OHM+OHM+OMS+PAPA+RISE+ROME+SB+SDOG+SHARE+SOHM+SOHM+SPA+SPACE+SQUID+TAC+TEMPLE+TIME+TOB+USDX+VSQ+WAGMI+WSOHM+XAMP+XDEF2+XEUS+Z2O</t>
+  </si>
+  <si>
+    <t>debug</t>
+  </si>
+  <si>
     <t>max</t>
   </si>
   <si>
-    <t>$BASED+3DOG+AMPL+AUSCM+BASE+BTRFLY+CHEEZ+CLAM+COIL+CROWN+DEBASE+DIGG+DIOS+DITTO+EIGHT+EXOD+FHM+FLOKIN+FOREVERPUMP+FORT+GRM+GRPL+GRV+GRX+GURU+GYRO+HEC+IN+IUP+JADE+KLIMA+LOVE+MARK+META+NMS+OHM+OHM+OMS+PAPA+RISE+ROME+SB+SDOG+SHARE+SOHM+SOHM+SPA+SPACE+SQUID+TAC+TEMPLE+TIME+TOB+USDX+VSQ+WAGMI+WSOHM+XAMP+XDEF2+XEUS+Z2O</t>
+    <t>max volume/open interest share</t>
   </si>
 </sst>
 </file>
@@ -444,13 +447,13 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -494,10 +497,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -508,7 +511,7 @@
         <v>0.1</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -532,7 +535,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>2.0000000000000001E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -540,7 +543,10 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.75</v>
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,7 +554,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
@@ -567,7 +573,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
security. Needs api_param offline file.
</commit_message>
<xml_diff>
--- a/DerivativeArbitrage/Runtime/configs/static_params.xlsx
+++ b/DerivativeArbitrage/Runtime/configs/static_params.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\pyCharmProjects\SystematicCeFi\DerivativeArbitrage\Runtime\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E234E3B-A68C-4C89-9603-7D1EB57579D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF94DB8-760D-48BE-99C0-5B11E81F3DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14925" yWindow="2145" windowWidth="23685" windowHeight="18180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22485" yWindow="1050" windowWidth="23685" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
     <sheet name="used" sheetId="2" r:id="rId2"/>
     <sheet name="saved" sheetId="3" r:id="rId3"/>
+    <sheet name="api" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="128">
   <si>
     <t>value</t>
   </si>
@@ -87,9 +89,6 @@
   </si>
   <si>
     <t>TYPE_ALLOWED</t>
-  </si>
-  <si>
-    <t>perpetual</t>
   </si>
   <si>
     <t>2h</t>
@@ -381,6 +380,48 @@
   </si>
   <si>
     <t>SysPerp</t>
+  </si>
+  <si>
+    <t>ftx</t>
+  </si>
+  <si>
+    <t>gAAAAABiYSBVmWSEPO3CdSv9MP4b0iW9fCENxGeVxFp5bocvcf72VrK-QmhYUWi4lyYguE4CHxqxVms2vMZYQX6rdrU5yxT2x_ciQggP4f6RaedcRXGZpbh3L7eZ0dpSUiP49L6ekn87</t>
+  </si>
+  <si>
+    <t>gAAAAABiYSaDXzyDtsop3smW8RDpYAEuR5JNMxfsTqk5EicPCVUterFS2kdfAGVZV6t7gH8oIJ0PRsw8t8kw2jqbNrldLciF87fyf2RXoBE4vFz9tXxhruv80oRyu27HR5EBeMiBZw-kuBdtjDesow5pE5hWiubfOrZwsXh6USzx7UGiaT7cE8o=</t>
+  </si>
+  <si>
+    <t>binance</t>
+  </si>
+  <si>
+    <t>okex5</t>
+  </si>
+  <si>
+    <t>huobi</t>
+  </si>
+  <si>
+    <t>deribit</t>
+  </si>
+  <si>
+    <t>kucoin</t>
+  </si>
+  <si>
+    <t>gAAAAABiYScDDwB0lKQmRppTVDZShd5ci7nQ90md9mdWQJ_mYuFMEAfcGEcF5OSk47rGkcJ4r8i4onB45MiRfq0_EaLyI5wD5HOH0uvzUBwu1oAouKY65bFWfA-hE-rsUZz8zYe6uQhf</t>
+  </si>
+  <si>
+    <t>gAAAAABiYScV10mFsmW6r9FPmqpYnVq15at3CGD9YI144DlB89q36C2Sq-tJUVNzsri0zoGn0NDvlPEeEzTNMlgDVuTJXivYto-5GNnz5bsmj935BqWjVns=</t>
+  </si>
+  <si>
+    <t>gAAAAABiYSczWAgnSfodcexldZ4HNAz88ZmB6fqRIAkjKCB7hkqjD6NOWLb552cW3j72qJWX12OONJ1LuBfjGqMNhE4pjaCgP5YGMarKAcsC1P5YKOp9-iPgMhPhi6YXsQWWXenTkwk2</t>
+  </si>
+  <si>
+    <t>gAAAAABiYSdCAg7WS0xMikO1-w0dM8n5bRlYCR3aThpyjyfDnMDOQRiuerAsy4pTMce0OurDCzlu4oZAXU5TVQfAN0P-WSP0AB1kCJK_aiFdl6mQrm4iA8XESzK-icqot6GkZdv5Pvn1</t>
+  </si>
+  <si>
+    <t>gAAAAABiYSdY_v0HSh583XP78S_WHFXPR9RC8jRUS17H5cC4_1E9yY3gTPnIfCsYCDxhxVNIGL8wdb_CcM6om_WHm-6Kvaut61DonvSoB8IVDeIAVll0MUZ_HjGT0hOODD6MQ6IDBIwR</t>
+  </si>
+  <si>
+    <t>perpetual+</t>
   </si>
 </sst>
 </file>
@@ -753,10 +794,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,9 +825,7 @@
       <c r="B2">
         <v>3</v>
       </c>
-      <c r="F2" s="10">
-        <v>44748</v>
-      </c>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -809,10 +848,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -823,7 +862,7 @@
         <v>0.05</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -831,7 +870,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -839,7 +878,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -858,37 +897,37 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12">
         <v>0.05</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,7 +935,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -915,7 +954,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -923,7 +962,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -931,22 +970,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f>0.000014*24*365.25</f>
-        <v>0.122724</v>
-      </c>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33">
-        <f>22*24/700</f>
-        <v>0.75428571428571434</v>
       </c>
     </row>
   </sheetData>
@@ -960,9 +987,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H1999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -973,16 +998,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -36966,9 +36991,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D79"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -36979,21 +37002,21 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="4">
         <v>7.0000000000000007E-2</v>
@@ -37009,7 +37032,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="4">
         <v>3.7499999999999999E-2</v>
@@ -37024,7 +37047,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="4">
         <v>0.06</v>
@@ -37038,7 +37061,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="4">
         <v>0.15</v>
@@ -37052,7 +37075,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="4">
         <v>4.7500000000000001E-2</v>
@@ -37067,7 +37090,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" s="4">
         <v>0.03</v>
@@ -37082,7 +37105,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="4">
         <v>3.5000000000000003E-2</v>
@@ -37096,7 +37119,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="4">
         <v>0.1</v>
@@ -37110,7 +37133,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="4">
         <v>0.1</v>
@@ -37124,7 +37147,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="4">
         <v>0.2</v>
@@ -37138,7 +37161,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="4">
         <v>3.0000000000000006E-2</v>
@@ -37152,7 +37175,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B13" s="4">
         <v>3.7499999999999999E-2</v>
@@ -37166,7 +37189,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="4">
         <v>3.4999999999999996E-2</v>
@@ -37180,7 +37203,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" s="4">
         <v>4.7500000000000007E-2</v>
@@ -37194,7 +37217,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="4">
         <v>0.1</v>
@@ -37208,7 +37231,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="4">
         <v>3.9999999999999987E-2</v>
@@ -37222,7 +37245,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="4">
         <v>0.01</v>
@@ -37236,7 +37259,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" s="4">
         <v>7.4999999999999997E-2</v>
@@ -37250,7 +37273,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B20" s="4">
         <v>5.000000000000001E-2</v>
@@ -37264,7 +37287,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="4">
         <v>3.7499999999999999E-2</v>
@@ -37278,7 +37301,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="4">
         <v>7.4999999999999997E-2</v>
@@ -37292,7 +37315,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="4">
         <v>2.2499999999999999E-2</v>
@@ -37306,7 +37329,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B24" s="4">
         <v>1.9999999999999997E-2</v>
@@ -37320,7 +37343,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="4">
         <v>0.11</v>
@@ -37334,7 +37357,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="4">
         <v>0.05</v>
@@ -37348,7 +37371,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27" s="4">
         <v>6.0000000000000005E-2</v>
@@ -37362,7 +37385,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="4">
         <v>0.08</v>
@@ -37376,7 +37399,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="4">
         <v>0.01</v>
@@ -37390,7 +37413,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="4">
         <v>9.9999999999999978E-2</v>
@@ -37404,7 +37427,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B31" s="4">
         <v>0.09</v>
@@ -37418,7 +37441,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="4">
         <v>4.4999999999999998E-2</v>
@@ -37432,7 +37455,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="4">
         <v>1.9999999999999997E-2</v>
@@ -37446,7 +37469,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="4">
         <v>5.7500000000000002E-2</v>
@@ -37460,7 +37483,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="4">
         <v>0.05</v>
@@ -37474,7 +37497,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B36" s="4">
         <v>7.0000000000000007E-2</v>
@@ -37488,7 +37511,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" s="4">
         <v>0.05</v>
@@ -37502,7 +37525,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="4">
         <v>0.06</v>
@@ -37516,7 +37539,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" s="4">
         <v>0.03</v>
@@ -37530,7 +37553,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="4">
         <v>0.02</v>
@@ -37544,7 +37567,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B41" s="4">
         <v>2.9999999999999992E-2</v>
@@ -37558,7 +37581,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B42" s="4">
         <v>3.9999999999999987E-2</v>
@@ -37572,7 +37595,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="4">
         <v>3.5000000000000003E-2</v>
@@ -37586,7 +37609,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B44" s="4">
         <v>7.0000000000000007E-2</v>
@@ -37600,7 +37623,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" s="4">
         <v>2.5000000000000001E-2</v>
@@ -37614,7 +37637,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" s="4">
         <v>5.5E-2</v>
@@ -37628,7 +37651,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" s="4">
         <v>0.04</v>
@@ -37642,7 +37665,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" s="4">
         <v>3.7499999999999999E-2</v>
@@ -37656,7 +37679,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B49" s="4">
         <v>0.03</v>
@@ -37670,7 +37693,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" s="4">
         <v>0.05</v>
@@ -37684,7 +37707,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" s="4">
         <v>0.08</v>
@@ -37698,7 +37721,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" s="4">
         <v>3.9999999999999987E-2</v>
@@ -37712,7 +37735,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="4">
         <v>0.05</v>
@@ -37726,7 +37749,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="4">
         <v>5.000000000000001E-2</v>
@@ -37740,7 +37763,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55" s="4">
         <v>5.000000000000001E-2</v>
@@ -37754,7 +37777,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B56" s="4">
         <v>3.9999999999999987E-2</v>
@@ -37768,7 +37791,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B57" s="4">
         <v>4.4999999999999998E-2</v>
@@ -37782,7 +37805,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B58" s="4">
         <v>3.9999999999999987E-2</v>
@@ -37796,7 +37819,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B59" s="4">
         <v>0.06</v>
@@ -37810,7 +37833,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B60" s="4">
         <v>1.9999999999999997E-2</v>
@@ -37824,7 +37847,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B61" s="4">
         <v>3.0000000000000006E-2</v>
@@ -37838,7 +37861,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B62" s="4">
         <v>4.5000000000000005E-2</v>
@@ -37852,7 +37875,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B63" s="4">
         <v>0.08</v>
@@ -37866,7 +37889,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B64" s="4">
         <v>0.03</v>
@@ -37880,7 +37903,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B65" s="4">
         <v>7.0000000000000007E-2</v>
@@ -37894,7 +37917,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B66" s="4">
         <v>0.04</v>
@@ -37909,7 +37932,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B67" s="4">
         <v>4.2500000000000003E-2</v>
@@ -37923,7 +37946,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B68" s="4">
         <v>6.25E-2</v>
@@ -37937,7 +37960,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B69" s="4">
         <v>6.25E-2</v>
@@ -37951,7 +37974,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B70" s="4">
         <v>7.0000000000000007E-2</v>
@@ -37965,7 +37988,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B71" s="4">
         <v>0.01</v>
@@ -37979,7 +38002,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B72" s="4">
         <v>0.01</v>
@@ -37993,7 +38016,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B73" s="4">
         <v>0.03</v>
@@ -38007,7 +38030,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B74" s="4">
         <v>2.5000000000000001E-2</v>
@@ -38021,7 +38044,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B75" s="4">
         <v>4.2500000000000003E-2</v>
@@ -38035,7 +38058,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" s="4">
         <v>0.06</v>
@@ -38049,7 +38072,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B77" s="4">
         <v>0.03</v>
@@ -38063,7 +38086,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B78" s="4">
         <v>2.75E-2</v>
@@ -38077,7 +38100,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B79" s="4">
         <v>3.5000000000000003E-2</v>
@@ -38093,4 +38116,84 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD8575F-0154-4AD6-A39D-B77BFF12CEE1}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added few encrypted keys
</commit_message>
<xml_diff>
--- a/DerivativeArbitrage/Runtime/configs/static_params.xlsx
+++ b/DerivativeArbitrage/Runtime/configs/static_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\pyCharmProjects\SystematicCeFi\DerivativeArbitrage\Runtime\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF94DB8-760D-48BE-99C0-5B11E81F3DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C11A5EC-C69A-4313-B61F-C5207F4F6C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22485" yWindow="1050" windowWidth="23685" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6135" yWindow="2385" windowWidth="45375" windowHeight="18180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="api" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="132">
   <si>
     <t>value</t>
   </si>
@@ -423,6 +422,18 @@
   <si>
     <t>perpetual+</t>
   </si>
+  <si>
+    <t>genesisvolatility</t>
+  </si>
+  <si>
+    <t>gAAAAABiYeo_C9OrcGR2cLESKhZJEp3scF6tAUjhaq7bWyFr_ZxDv_UjyJC5lh57av3yht3G2AVBc-qL0gNvttVcvOSVbt5jcJ68KBaojQbc5be2kGTKIsM=</t>
+  </si>
+  <si>
+    <t>paradigm</t>
+  </si>
+  <si>
+    <t>lRg/osd9fin+U8WmttU1trbyvb2UA8LBoqmhZpDGO9NOFHS6</t>
+  </si>
 </sst>
 </file>
 
@@ -796,8 +807,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +905,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -916,7 +927,7 @@
         <v>109</v>
       </c>
       <c r="B12">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C12" t="s">
         <v>110</v>
@@ -38120,14 +38131,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD8575F-0154-4AD6-A39D-B77BFF12CEE1}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -38193,7 +38205,24 @@
         <v>126</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all dates are utc (reset to None before exel dump)
</commit_message>
<xml_diff>
--- a/DerivativeArbitrage/Runtime/configs/static_params.xlsx
+++ b/DerivativeArbitrage/Runtime/configs/static_params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\pyCharmProjects\SystematicCeFi\DerivativeArbitrage\Runtime\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD83AE83-F395-4CA7-9DBC-6717CA971181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511A06DF-5485-411C-AD89-08F77B4FA2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4485" yWindow="525" windowWidth="45375" windowHeight="18180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4635" yWindow="1260" windowWidth="22380" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -372,15 +372,6 @@
     <t>screens out low carry underlyings</t>
   </si>
   <si>
-    <t>wide</t>
-  </si>
-  <si>
-    <t>OMG+</t>
-  </si>
-  <si>
-    <t>SysPerp</t>
-  </si>
-  <si>
     <t>ftx</t>
   </si>
   <si>
@@ -433,6 +424,15 @@
   </si>
   <si>
     <t>gAAAAABiYyC0xNDHHY5FzK8QKEZO85aIFBb8KyhNnXPKfXHqFhR1hr3dZP6A2yCz9Ez79q9AIB_KM-_jMRSOsAeuBRWycJSCxPd9U4krer6Kc-BkazWRiFH8Vwvh-Z6G6pNRLZ2_fkO-h2lM3RK9nPVIJAEybLCSbQ==</t>
+  </si>
+  <si>
+    <t>UST+</t>
+  </si>
+  <si>
+    <t>SysPerp</t>
+  </si>
+  <si>
+    <t>wide</t>
   </si>
 </sst>
 </file>
@@ -807,8 +807,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +859,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -946,7 +946,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -965,7 +965,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -973,7 +973,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -38133,7 +38133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD8575F-0154-4AD6-A39D-B77BFF12CEE1}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -38156,69 +38156,69 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>